<commit_message>
assigned templates to DataPLANT
</commit_message>
<xml_diff>
--- a/templates/dataplant/MIAPPE_experimental_factors.xlsx
+++ b/templates/dataplant/MIAPPE_experimental_factors.xlsx
@@ -1,11 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26220"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="1541" documentId="11_92483E2D04E89AD36523F29B863E8C1851038389" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3989C30E-EA1E-42B2-9B4B-A87CA2F155BD}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stella Eggels\Documents\GitHub\Swate-templates\templates\dataplant\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{645C685A-8365-4D6F-8193-1CA3E8F228AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="experimental_factors" sheetId="1" r:id="rId1"/>
@@ -121,7 +126,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="191">
   <si>
     <t>Source Name</t>
   </si>
@@ -582,9 +587,6 @@
     <t>Version</t>
   </si>
   <si>
-    <t>1.0.0</t>
-  </si>
-  <si>
     <t>Description</t>
   </si>
   <si>
@@ -691,13 +693,19 @@
   </si>
   <si>
     <t>Authors Role Term Source REF</t>
+  </si>
+  <si>
+    <t>DataPLANT</t>
+  </si>
+  <si>
+    <t>1.0.1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -888,7 +896,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" xr:uid="{00000000-000B-0000-0000-000008000000}"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="50">
     <dxf>
@@ -1480,91 +1488,91 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BY4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="76" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="32.85546875" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="39.7109375" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="119.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="32.85546875" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="39.7109375" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="112.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="32.85546875" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="39.7109375" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="32.88671875" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="39.6640625" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="119.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="32.88671875" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="39.6640625" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="112.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="32.88671875" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="39.6640625" hidden="1" customWidth="1"/>
     <col min="11" max="11" width="31" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="32.85546875" hidden="1" customWidth="1"/>
-    <col min="13" max="13" width="39.7109375" hidden="1" customWidth="1"/>
-    <col min="14" max="14" width="26.7109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="32.85546875" hidden="1" customWidth="1"/>
-    <col min="16" max="16" width="39.7109375" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="33.28515625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="32.85546875" hidden="1" customWidth="1"/>
-    <col min="19" max="19" width="39.7109375" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="32.88671875" hidden="1" customWidth="1"/>
+    <col min="13" max="13" width="39.6640625" hidden="1" customWidth="1"/>
+    <col min="14" max="14" width="26.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="32.88671875" hidden="1" customWidth="1"/>
+    <col min="16" max="16" width="39.6640625" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="33.33203125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="32.88671875" hidden="1" customWidth="1"/>
+    <col min="19" max="19" width="39.6640625" hidden="1" customWidth="1"/>
     <col min="20" max="20" width="26" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="32.85546875" hidden="1" customWidth="1"/>
-    <col min="22" max="22" width="39.7109375" hidden="1" customWidth="1"/>
-    <col min="23" max="23" width="25.85546875" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="32.85546875" hidden="1" customWidth="1"/>
-    <col min="25" max="25" width="39.7109375" hidden="1" customWidth="1"/>
-    <col min="26" max="26" width="26.42578125" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="32.85546875" hidden="1" customWidth="1"/>
-    <col min="28" max="28" width="39.7109375" hidden="1" customWidth="1"/>
-    <col min="29" max="29" width="25.5703125" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="32.85546875" hidden="1" customWidth="1"/>
-    <col min="31" max="31" width="39.7109375" hidden="1" customWidth="1"/>
-    <col min="32" max="32" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="32.85546875" hidden="1" customWidth="1"/>
-    <col min="34" max="34" width="39.7109375" hidden="1" customWidth="1"/>
-    <col min="35" max="35" width="31.42578125" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="32.85546875" hidden="1" customWidth="1"/>
-    <col min="37" max="37" width="39.7109375" hidden="1" customWidth="1"/>
-    <col min="38" max="38" width="26.5703125" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="32.85546875" hidden="1" customWidth="1"/>
-    <col min="40" max="40" width="39.7109375" hidden="1" customWidth="1"/>
-    <col min="41" max="41" width="31.28515625" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="32.85546875" hidden="1" customWidth="1"/>
-    <col min="43" max="43" width="39.7109375" hidden="1" customWidth="1"/>
-    <col min="44" max="44" width="26.140625" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="32.85546875" hidden="1" customWidth="1"/>
-    <col min="46" max="46" width="39.7109375" hidden="1" customWidth="1"/>
-    <col min="47" max="47" width="27.42578125" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="32.85546875" hidden="1" customWidth="1"/>
-    <col min="49" max="49" width="39.7109375" hidden="1" customWidth="1"/>
-    <col min="50" max="50" width="44.140625" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="32.85546875" hidden="1" customWidth="1"/>
-    <col min="52" max="52" width="39.7109375" hidden="1" customWidth="1"/>
-    <col min="53" max="53" width="24.7109375" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="32.85546875" hidden="1" customWidth="1"/>
-    <col min="55" max="55" width="39.7109375" hidden="1" customWidth="1"/>
-    <col min="56" max="56" width="21.140625" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="32.85546875" hidden="1" customWidth="1"/>
-    <col min="58" max="58" width="39.7109375" hidden="1" customWidth="1"/>
-    <col min="59" max="59" width="26.28515625" bestFit="1" customWidth="1"/>
-    <col min="60" max="60" width="32.85546875" hidden="1" customWidth="1"/>
-    <col min="61" max="61" width="39.7109375" hidden="1" customWidth="1"/>
-    <col min="62" max="62" width="35.7109375" bestFit="1" customWidth="1"/>
-    <col min="63" max="63" width="32.85546875" hidden="1" customWidth="1"/>
-    <col min="64" max="64" width="39.7109375" hidden="1" customWidth="1"/>
-    <col min="65" max="65" width="31.7109375" bestFit="1" customWidth="1"/>
-    <col min="66" max="66" width="32.85546875" hidden="1" customWidth="1"/>
-    <col min="67" max="67" width="39.7109375" hidden="1" customWidth="1"/>
+    <col min="21" max="21" width="32.88671875" hidden="1" customWidth="1"/>
+    <col min="22" max="22" width="39.6640625" hidden="1" customWidth="1"/>
+    <col min="23" max="23" width="25.88671875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="32.88671875" hidden="1" customWidth="1"/>
+    <col min="25" max="25" width="39.6640625" hidden="1" customWidth="1"/>
+    <col min="26" max="26" width="26.44140625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="32.88671875" hidden="1" customWidth="1"/>
+    <col min="28" max="28" width="39.6640625" hidden="1" customWidth="1"/>
+    <col min="29" max="29" width="25.5546875" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="32.88671875" hidden="1" customWidth="1"/>
+    <col min="31" max="31" width="39.6640625" hidden="1" customWidth="1"/>
+    <col min="32" max="32" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="32.88671875" hidden="1" customWidth="1"/>
+    <col min="34" max="34" width="39.6640625" hidden="1" customWidth="1"/>
+    <col min="35" max="35" width="31.44140625" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="32.88671875" hidden="1" customWidth="1"/>
+    <col min="37" max="37" width="39.6640625" hidden="1" customWidth="1"/>
+    <col min="38" max="38" width="26.5546875" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="32.88671875" hidden="1" customWidth="1"/>
+    <col min="40" max="40" width="39.6640625" hidden="1" customWidth="1"/>
+    <col min="41" max="41" width="31.33203125" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="32.88671875" hidden="1" customWidth="1"/>
+    <col min="43" max="43" width="39.6640625" hidden="1" customWidth="1"/>
+    <col min="44" max="44" width="26.109375" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="32.88671875" hidden="1" customWidth="1"/>
+    <col min="46" max="46" width="39.6640625" hidden="1" customWidth="1"/>
+    <col min="47" max="47" width="27.44140625" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="32.88671875" hidden="1" customWidth="1"/>
+    <col min="49" max="49" width="39.6640625" hidden="1" customWidth="1"/>
+    <col min="50" max="50" width="44.109375" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="32.88671875" hidden="1" customWidth="1"/>
+    <col min="52" max="52" width="39.6640625" hidden="1" customWidth="1"/>
+    <col min="53" max="53" width="24.6640625" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="32.88671875" hidden="1" customWidth="1"/>
+    <col min="55" max="55" width="39.6640625" hidden="1" customWidth="1"/>
+    <col min="56" max="56" width="21.109375" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="32.88671875" hidden="1" customWidth="1"/>
+    <col min="58" max="58" width="39.6640625" hidden="1" customWidth="1"/>
+    <col min="59" max="59" width="26.33203125" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="32.88671875" hidden="1" customWidth="1"/>
+    <col min="61" max="61" width="39.6640625" hidden="1" customWidth="1"/>
+    <col min="62" max="62" width="35.6640625" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="32.88671875" hidden="1" customWidth="1"/>
+    <col min="64" max="64" width="39.6640625" hidden="1" customWidth="1"/>
+    <col min="65" max="65" width="31.6640625" bestFit="1" customWidth="1"/>
+    <col min="66" max="66" width="32.88671875" hidden="1" customWidth="1"/>
+    <col min="67" max="67" width="39.6640625" hidden="1" customWidth="1"/>
     <col min="68" max="68" width="26" bestFit="1" customWidth="1"/>
-    <col min="69" max="69" width="32.85546875" hidden="1" customWidth="1"/>
-    <col min="70" max="70" width="39.7109375" hidden="1" customWidth="1"/>
-    <col min="71" max="71" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="72" max="72" width="33.28515625" hidden="1" customWidth="1"/>
-    <col min="73" max="73" width="40.140625" hidden="1" customWidth="1"/>
+    <col min="69" max="69" width="32.88671875" hidden="1" customWidth="1"/>
+    <col min="70" max="70" width="39.6640625" hidden="1" customWidth="1"/>
+    <col min="71" max="71" width="20.44140625" bestFit="1" customWidth="1"/>
+    <col min="72" max="72" width="33.33203125" hidden="1" customWidth="1"/>
+    <col min="73" max="73" width="40.109375" hidden="1" customWidth="1"/>
     <col min="74" max="74" width="29" bestFit="1" customWidth="1"/>
     <col min="75" max="76" width="0" hidden="1" customWidth="1"/>
-    <col min="77" max="77" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="77" max="77" width="15.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:77">
+    <row r="1" spans="1:77" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1797,7 +1805,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="2" spans="1:77">
+    <row r="2" spans="1:77" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>77</v>
       </c>
@@ -1920,7 +1928,7 @@
       <c r="BW2" s="1"/>
       <c r="BX2" s="1"/>
     </row>
-    <row r="3" spans="1:77">
+    <row r="3" spans="1:77" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>101</v>
       </c>
@@ -2043,7 +2051,7 @@
       <c r="BW3" s="1"/>
       <c r="BX3" s="1"/>
     </row>
-    <row r="4" spans="1:77">
+    <row r="4" spans="1:77" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>125</v>
       </c>
@@ -2180,17 +2188,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59D5CDEF-907C-4DD9-85AD-7F9C87E1B2BA}">
   <dimension ref="A1:D27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="35" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="57.140625" customWidth="1"/>
+    <col min="2" max="2" width="57.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>148</v>
       </c>
@@ -2198,7 +2206,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>150</v>
       </c>
@@ -2206,187 +2214,189 @@
         <v>151</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>152</v>
       </c>
       <c r="B3" s="9" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="5" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" ht="50.25" customHeight="1">
-      <c r="A4" s="5" t="s">
+      <c r="B4" s="9" t="s">
         <v>154</v>
       </c>
-      <c r="B4" s="9" t="s">
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="5" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5" s="5" t="s">
+      <c r="B5" s="9" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="5" t="s">
         <v>156</v>
       </c>
-      <c r="B5" s="9"/>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" s="5" t="s">
+      <c r="B6" s="9" t="s">
         <v>157</v>
       </c>
-      <c r="B6" s="9" t="s">
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="6" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7" s="6" t="s">
+      <c r="B7" s="10"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="5" t="s">
         <v>159</v>
       </c>
-      <c r="B7" s="10"/>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="A8" s="5" t="s">
+      <c r="B8" s="11"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="5" t="s">
         <v>160</v>
       </c>
-      <c r="B8" s="11"/>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="A9" s="5" t="s">
+      <c r="B9" s="9"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="5" t="s">
         <v>161</v>
       </c>
-      <c r="B9" s="9"/>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="A10" s="5" t="s">
+      <c r="B10" s="9"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" s="6" t="s">
         <v>162</v>
       </c>
-      <c r="B10" s="9"/>
-    </row>
-    <row r="11" spans="1:4">
-      <c r="A11" s="6" t="s">
+      <c r="B11" s="10"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" s="5" t="s">
         <v>163</v>
       </c>
-      <c r="B11" s="10"/>
-    </row>
-    <row r="12" spans="1:4">
-      <c r="A12" s="5" t="s">
+      <c r="B12" s="11" t="s">
         <v>164</v>
       </c>
-      <c r="B12" s="11" t="s">
+      <c r="C12" t="s">
         <v>165</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
         <v>166</v>
       </c>
-      <c r="D12" t="s">
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" s="5" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="13" spans="1:4">
-      <c r="A13" s="5" t="s">
+      <c r="B13" s="9"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" s="5" t="s">
         <v>168</v>
       </c>
-      <c r="B13" s="9"/>
-    </row>
-    <row r="14" spans="1:4">
-      <c r="A14" s="5" t="s">
+      <c r="B14" s="9"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" s="6" t="s">
         <v>169</v>
       </c>
-      <c r="B14" s="9"/>
-    </row>
-    <row r="15" spans="1:4">
-      <c r="A15" s="6" t="s">
+      <c r="B15" s="10"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" s="5" t="s">
         <v>170</v>
       </c>
-      <c r="B15" s="10"/>
-    </row>
-    <row r="16" spans="1:4">
-      <c r="A16" s="5" t="s">
+      <c r="B16" s="11" t="s">
         <v>171</v>
       </c>
-      <c r="B16" s="11" t="s">
+      <c r="C16" t="s">
         <v>172</v>
       </c>
-      <c r="C16" t="s">
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" s="5" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="17" spans="1:3">
-      <c r="A17" s="5" t="s">
+      <c r="B17" s="9" t="s">
         <v>174</v>
       </c>
-      <c r="B17" s="9" t="s">
+      <c r="C17" t="s">
         <v>175</v>
       </c>
-      <c r="C17" t="s">
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" s="5" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="18" spans="1:3">
-      <c r="A18" s="5" t="s">
+      <c r="B18" s="9"/>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" s="5" t="s">
         <v>177</v>
       </c>
-      <c r="B18" s="9"/>
-    </row>
-    <row r="19" spans="1:3">
-      <c r="A19" s="5" t="s">
+      <c r="B19" s="13" t="s">
         <v>178</v>
       </c>
-      <c r="B19" s="13" t="s">
+      <c r="C19" s="14" t="s">
         <v>179</v>
       </c>
-      <c r="C19" s="14" t="s">
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" s="5" t="s">
         <v>180</v>
       </c>
-    </row>
-    <row r="20" spans="1:3">
-      <c r="A20" s="5" t="s">
+      <c r="B20" s="9"/>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" s="5" t="s">
         <v>181</v>
       </c>
-      <c r="B20" s="9"/>
-    </row>
-    <row r="21" spans="1:3">
-      <c r="A21" s="5" t="s">
+      <c r="B21" s="9"/>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" s="5" t="s">
         <v>182</v>
       </c>
-      <c r="B21" s="9"/>
-    </row>
-    <row r="22" spans="1:3">
-      <c r="A22" s="5" t="s">
+      <c r="B22" s="9"/>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" s="5" t="s">
         <v>183</v>
       </c>
-      <c r="B22" s="9"/>
-    </row>
-    <row r="23" spans="1:3">
-      <c r="A23" s="5" t="s">
+      <c r="B23" s="9" t="s">
         <v>184</v>
       </c>
-      <c r="B23" s="9" t="s">
+      <c r="C23" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" s="5" t="s">
         <v>185</v>
       </c>
-      <c r="C23" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3">
-      <c r="A24" s="5" t="s">
+      <c r="B24" s="9"/>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25" s="5" t="s">
         <v>186</v>
       </c>
-      <c r="B24" s="9"/>
-    </row>
-    <row r="25" spans="1:3">
-      <c r="A25" s="5" t="s">
+      <c r="B25" s="9"/>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26" s="5" t="s">
         <v>187</v>
       </c>
-      <c r="B25" s="9"/>
-    </row>
-    <row r="26" spans="1:3">
-      <c r="A26" s="5" t="s">
+      <c r="B26" s="9"/>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27" s="7" t="s">
         <v>188</v>
-      </c>
-      <c r="B26" s="9"/>
-    </row>
-    <row r="27" spans="1:3">
-      <c r="A27" s="7" t="s">
-        <v>189</v>
       </c>
       <c r="B27" s="12"/>
     </row>

</xml_diff>

<commit_message>
added missing ontology reference to building block
</commit_message>
<xml_diff>
--- a/templates/dataplant/MIAPPE_experimental_factors.xlsx
+++ b/templates/dataplant/MIAPPE_experimental_factors.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stella Eggels\sciebo - Eggels, Stella (s.eggels@fz-juelich.de)@fz-juelich.sciebo.de\SE\DataPLANT\ARCs und SWATE\Ersatz fehlerhafter MIAPPE templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stella Eggels\Documents\GitHub\Swate-templates\templates\dataplant\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FE0CDED-F8D2-41F3-92D5-A71445506929}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF0223BB-AA5B-4DB1-8AB3-F7199BC83CA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{FF43168E-BF1D-403E-A0C6-C66E124CD6A8}"/>
   </bookViews>
@@ -356,15 +356,6 @@
     <t>Term Accession Number (MIAPPE:0165)</t>
   </si>
   <si>
-    <t>Factor [other perturbation]</t>
-  </si>
-  <si>
-    <t>Term Source REF ()</t>
-  </si>
-  <si>
-    <t>Term Accession Number ()</t>
-  </si>
-  <si>
     <t>Id</t>
   </si>
   <si>
@@ -452,9 +443,6 @@
     <t>MIAPPE experimental factors</t>
   </si>
   <si>
-    <t>1.0.2</t>
-  </si>
-  <si>
     <t>Template that includes all experimental factors from the MIAPPE appendix.</t>
   </si>
   <si>
@@ -501,6 +489,18 @@
   </si>
   <si>
     <t>Forschungszentrum Jülich</t>
+  </si>
+  <si>
+    <t>Factor [Other perturbation]</t>
+  </si>
+  <si>
+    <t>Term Source REF (MIAPPE:0166)</t>
+  </si>
+  <si>
+    <t>Term Accession Number (MIAPPE:0166)</t>
+  </si>
+  <si>
+    <t>1.0.3</t>
   </si>
 </sst>
 </file>
@@ -1008,9 +1008,9 @@
     <tableColumn id="72" xr3:uid="{38210844-DC37-4812-9F08-BA5AE8937215}" name="Parameter [pH regime]" dataDxfId="5"/>
     <tableColumn id="73" xr3:uid="{C417BF99-301F-42DA-925A-3B04D7D2A7B5}" name="Term Source REF (MIAPPE:0165)" dataDxfId="4"/>
     <tableColumn id="74" xr3:uid="{F35D3DF1-B937-460F-8185-48FBE0879813}" name="Term Accession Number (MIAPPE:0165)" dataDxfId="3"/>
-    <tableColumn id="75" xr3:uid="{1F3522D5-899E-45E6-9E61-803510067772}" name="Factor [other perturbation]" dataDxfId="2"/>
-    <tableColumn id="76" xr3:uid="{9534B68D-A0B7-45E6-8332-BBAFB0B72EE9}" name="Term Source REF ()" dataDxfId="1"/>
-    <tableColumn id="77" xr3:uid="{36F2EF85-2D4F-410C-837B-1E8C5CCAA9EF}" name="Term Accession Number ()" dataDxfId="0"/>
+    <tableColumn id="75" xr3:uid="{4AAAFC0F-A2FC-4338-884D-40ED0245B78A}" name="Factor [Other perturbation]" dataDxfId="2"/>
+    <tableColumn id="76" xr3:uid="{0AF69FC2-3CE7-4B14-828D-D58536CA42BA}" name="Term Source REF (MIAPPE:0166)" dataDxfId="1"/>
+    <tableColumn id="77" xr3:uid="{7DC8F0AC-5E9E-4579-AAB8-12B7A370BD83}" name="Term Accession Number (MIAPPE:0166)" dataDxfId="0"/>
     <tableColumn id="2" xr3:uid="{357E72D8-59B1-435C-87C3-487D0843404E}" name="Sample Name"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1349,7 +1349,7 @@
 
 <file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
 <wetp:taskpanes xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
-  <wetp:taskpane dockstate="right" visibility="0" width="438" row="2">
+  <wetp:taskpane dockstate="right" visibility="0" width="438" row="1">
     <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
   </wetp:taskpane>
 </wetp:taskpanes>
@@ -1369,8 +1369,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DDCA4005-715D-4C76-BB29-73EE133AC0E7}">
   <dimension ref="A1:BY2"/>
   <sheetViews>
-    <sheetView topLeftCell="BD1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView topLeftCell="BJ1" workbookViewId="0">
+      <selection activeCell="BV6" sqref="BV6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1448,9 +1448,9 @@
     <col min="71" max="71" width="22.44140625" bestFit="1" customWidth="1"/>
     <col min="72" max="72" width="30.6640625" hidden="1" customWidth="1"/>
     <col min="73" max="73" width="37.109375" hidden="1" customWidth="1"/>
-    <col min="74" max="74" width="26.109375" bestFit="1" customWidth="1"/>
-    <col min="75" max="75" width="19.109375" hidden="1" customWidth="1"/>
-    <col min="76" max="76" width="25.5546875" hidden="1" customWidth="1"/>
+    <col min="74" max="74" width="26.33203125" bestFit="1" customWidth="1"/>
+    <col min="75" max="75" width="30.6640625" hidden="1" customWidth="1"/>
+    <col min="76" max="76" width="37.109375" hidden="1" customWidth="1"/>
     <col min="77" max="77" width="14.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1675,13 +1675,13 @@
         <v>74</v>
       </c>
       <c r="BV1" t="s">
-        <v>75</v>
+        <v>120</v>
       </c>
       <c r="BW1" t="s">
-        <v>76</v>
+        <v>121</v>
       </c>
       <c r="BX1" t="s">
-        <v>77</v>
+        <v>122</v>
       </c>
       <c r="BY1" t="s">
         <v>1</v>
@@ -1925,7 +1925,7 @@
   <dimension ref="A1:D27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1937,215 +1937,215 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>107</v>
+        <v>123</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B7" s="8"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B8" s="9"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B9" s="7"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B10" s="7"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B11" s="8"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="C12" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="D12" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B13" s="7"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B14" s="7"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B15" s="8"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B16" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="C16" t="s">
+        <v>113</v>
+      </c>
+      <c r="D16" t="s">
         <v>114</v>
-      </c>
-      <c r="C16" t="s">
-        <v>117</v>
-      </c>
-      <c r="D16" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B17" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="C17" t="s">
+        <v>112</v>
+      </c>
+      <c r="D17" t="s">
         <v>115</v>
-      </c>
-      <c r="C17" t="s">
-        <v>116</v>
-      </c>
-      <c r="D17" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B18" s="7"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="C19" s="12" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="D19" s="12" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B20" s="7"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B21" s="7"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B22" s="7"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="C23" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="D23" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B24" s="7"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B25" s="7"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="B26" s="7"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" s="5" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="B27" s="10"/>
     </row>

</xml_diff>

<commit_message>
change ID in MIAPPE experimental factors template
</commit_message>
<xml_diff>
--- a/templates/dataplant/MIAPPE_experimental_factors.xlsx
+++ b/templates/dataplant/MIAPPE_experimental_factors.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stella Eggels\Documents\GitHub\Swate-templates\templates\dataplant\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF0223BB-AA5B-4DB1-8AB3-F7199BC83CA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{371C583E-20F3-4D01-903C-136AA0CB78FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{FF43168E-BF1D-403E-A0C6-C66E124CD6A8}"/>
   </bookViews>
@@ -437,9 +437,6 @@
     <t>Authors Role Term Source REF</t>
   </si>
   <si>
-    <t>96bb7d4a-74b0-4558-a5c8-8595ca64bf93</t>
-  </si>
-  <si>
     <t>MIAPPE experimental factors</t>
   </si>
   <si>
@@ -501,6 +498,9 @@
   </si>
   <si>
     <t>1.0.3</t>
+  </si>
+  <si>
+    <t>25a1a248-f9c0-4af4-b6d1-980b2dc8427d</t>
   </si>
 </sst>
 </file>
@@ -1675,13 +1675,13 @@
         <v>74</v>
       </c>
       <c r="BV1" t="s">
+        <v>119</v>
+      </c>
+      <c r="BW1" t="s">
         <v>120</v>
       </c>
-      <c r="BW1" t="s">
+      <c r="BX1" t="s">
         <v>121</v>
-      </c>
-      <c r="BX1" t="s">
-        <v>122</v>
       </c>
       <c r="BY1" t="s">
         <v>1</v>
@@ -1925,7 +1925,7 @@
   <dimension ref="A1:D27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1940,7 +1940,7 @@
         <v>75</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>102</v>
+        <v>123</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -1948,7 +1948,7 @@
         <v>76</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -1956,7 +1956,7 @@
         <v>77</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -1964,7 +1964,7 @@
         <v>78</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -1972,7 +1972,7 @@
         <v>79</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -1980,7 +1980,7 @@
         <v>80</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
@@ -2018,13 +2018,13 @@
         <v>86</v>
       </c>
       <c r="B12" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="C12" t="s">
         <v>107</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
         <v>108</v>
-      </c>
-      <c r="D12" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
@@ -2050,13 +2050,13 @@
         <v>90</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C16" t="s">
+        <v>112</v>
+      </c>
+      <c r="D16" t="s">
         <v>113</v>
-      </c>
-      <c r="D16" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
@@ -2064,13 +2064,13 @@
         <v>91</v>
       </c>
       <c r="B17" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="C17" t="s">
         <v>111</v>
       </c>
-      <c r="C17" t="s">
-        <v>112</v>
-      </c>
       <c r="D17" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
@@ -2084,13 +2084,13 @@
         <v>93</v>
       </c>
       <c r="B19" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="C19" s="12" t="s">
         <v>116</v>
       </c>
-      <c r="C19" s="12" t="s">
+      <c r="D19" s="12" t="s">
         <v>117</v>
-      </c>
-      <c r="D19" s="12" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
@@ -2116,13 +2116,13 @@
         <v>97</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C23" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D23" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>